<commit_message>
#8 Got that test passed
</commit_message>
<xml_diff>
--- a/apache-poi-filters/src/test/resources/input.xlsx
+++ b/apache-poi-filters/src/test/resources/input.xlsx
@@ -388,7 +388,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -442,7 +442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>

</xml_diff>